<commit_message>
commiting code 4th june
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/DownloadedFiles/Export Scheduler (1).xlsx
+++ b/ocms/src/test/resources/DownloadedFiles/Export Scheduler (1).xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -49,28 +49,37 @@
     <t xml:space="preserve">Last Changed On</t>
   </si>
   <si>
+    <t xml:space="preserve">Atr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00:03:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AuditTrailReport</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">EC2AMAZ-N8SAHHO\Administrator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/06/2021 17:24:49</t>
+  </si>
+  <si>
     <t xml:space="preserve">ExpSch1</t>
   </si>
   <si>
-    <t xml:space="preserve">test</t>
-  </si>
-  <si>
     <t xml:space="preserve">10:00:00</t>
   </si>
   <si>
-    <t xml:space="preserve">Daily</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AuditTrailReport</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">EC2AMAZ-N8SAHHO\Administrator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02/06/2021 17:12:29</t>
+    <t xml:space="preserve">03/06/2021 20:53:07</t>
   </si>
   <si>
     <t xml:space="preserve">ExpSch2</t>
@@ -82,7 +91,7 @@
     <t xml:space="preserve">Tuesday</t>
   </si>
   <si>
-    <t xml:space="preserve">02/06/2021 17:05:38</t>
+    <t xml:space="preserve">03/06/2021 20:46:18</t>
   </si>
   <si>
     <t xml:space="preserve">ExpSch3</t>
@@ -91,7 +100,7 @@
     <t xml:space="preserve">Monthly</t>
   </si>
   <si>
-    <t xml:space="preserve">02/06/2021 17:06:40</t>
+    <t xml:space="preserve">03/06/2021 20:47:16</t>
   </si>
   <si>
     <t xml:space="preserve">ExpSch4</t>
@@ -103,7 +112,7 @@
     <t xml:space="preserve">CustomDaily</t>
   </si>
   <si>
-    <t xml:space="preserve">02/06/2021 17:07:37</t>
+    <t xml:space="preserve">03/06/2021 20:48:11</t>
   </si>
 </sst>
 </file>
@@ -171,7 +180,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane state="frozen" ySplit="1" topLeftCell="A2"/>
@@ -263,51 +272,52 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
       </c>
       <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="2">
-             </c>
+      <c r="G4" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="H4" t="s">
         <v>16</v>
       </c>
@@ -326,28 +336,59 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="2">
+             </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="2" t="s">
+    </row>
+    <row r="6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>